<commit_message>
updated MyUF and excel file
</commit_message>
<xml_diff>
--- a/nVsTimeFastAnalysis.xlsx
+++ b/nVsTimeFastAnalysis.xlsx
@@ -6105,8 +6105,8 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>148167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
@@ -6584,7 +6584,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>